<commit_message>
taxi ranks data in Lisbon are available in geojson format
</commit_message>
<xml_diff>
--- a/data/Praças de Táxis Lisboa.xlsx
+++ b/data/Praças de Táxis Lisboa.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bc8396b9dd9ba2bd/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leono\Projetos\ICO_VRP\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7EA0CD35-AF42-4062-BA54-AD930019FC7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6652C2E-B63D-4D22-9C6D-39024C6271F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{E75CE120-6359-47BD-B546-9A1E0C4C2FA2}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{E75CE120-6359-47BD-B546-9A1E0C4C2FA2}"/>
   </bookViews>
   <sheets>
     <sheet name="Folha1" sheetId="1" r:id="rId1"/>
@@ -191,7 +191,7 @@
     <t>38.705393525148416</t>
   </si>
   <si>
-    <t xml:space="preserve"> '-9.227705326284289</t>
+    <t>-9.227705326284289</t>
   </si>
 </sst>
 </file>
@@ -566,8 +566,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6ACCD246-E9DC-4C11-A275-F19C63E92FAA}">
   <dimension ref="A1:C18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -771,7 +771,7 @@
       <c r="B18" t="s">
         <v>50</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" s="1" t="s">
         <v>51</v>
       </c>
     </row>

</xml_diff>